<commit_message>
Now manual setting for importing support entering column names!
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariusz\Desktop\Model lodowiska\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICE\ICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E14E29-5C31-45A4-AAA7-F3990477C7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C742EA-1AE6-4EFE-8939-B218718A628A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6852908-AD57-44F1-8DA2-95DC3E542023}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{D6852908-AD57-44F1-8DA2-95DC3E542023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Pon</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Niedz.</t>
-  </si>
-  <si>
-    <t>Temperatura nastawienia</t>
   </si>
   <si>
     <t>Temperatura na termometrze</t>
@@ -572,7 +569,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,32 +585,30 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>7</v>
-      </c>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -640,9 +635,7 @@
       <c r="H2" s="1">
         <v>80</v>
       </c>
-      <c r="I2" s="10">
-        <v>3</v>
-      </c>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -667,9 +660,7 @@
       <c r="H3" s="2">
         <v>70</v>
       </c>
-      <c r="I3" s="11">
-        <v>2</v>
-      </c>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -694,9 +685,7 @@
       <c r="H4" s="2">
         <v>30</v>
       </c>
-      <c r="I4" s="11">
-        <v>1</v>
-      </c>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -721,9 +710,7 @@
       <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" s="12">
-        <v>1</v>
-      </c>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -750,9 +737,7 @@
       <c r="H6" s="1">
         <v>80</v>
       </c>
-      <c r="I6" s="10">
-        <v>0</v>
-      </c>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -777,9 +762,7 @@
       <c r="H7" s="2">
         <v>70</v>
       </c>
-      <c r="I7" s="11">
-        <v>4.3</v>
-      </c>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -804,9 +787,7 @@
       <c r="H8" s="2">
         <v>30</v>
       </c>
-      <c r="I8" s="11">
-        <v>3.6</v>
-      </c>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -831,9 +812,7 @@
       <c r="H9" s="3">
         <v>40</v>
       </c>
-      <c r="I9" s="12">
-        <v>2.9</v>
-      </c>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -860,9 +839,7 @@
       <c r="H10" s="1">
         <v>80</v>
       </c>
-      <c r="I10" s="10">
-        <v>2.2000000000000002</v>
-      </c>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -887,9 +864,7 @@
       <c r="H11" s="2">
         <v>70</v>
       </c>
-      <c r="I11" s="11">
-        <v>1.5</v>
-      </c>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -914,9 +889,7 @@
       <c r="H12" s="2">
         <v>30</v>
       </c>
-      <c r="I12" s="11">
-        <v>0.79999999999999982</v>
-      </c>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -941,9 +914,7 @@
       <c r="H13" s="3">
         <v>40</v>
       </c>
-      <c r="I13" s="12">
-        <v>9.9999999999999645E-2</v>
-      </c>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -970,9 +941,7 @@
       <c r="H14" s="1">
         <v>80</v>
       </c>
-      <c r="I14" s="10">
-        <v>-0.59999999999999964</v>
-      </c>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -997,9 +966,7 @@
       <c r="H15" s="2">
         <v>70</v>
       </c>
-      <c r="I15" s="11">
-        <v>-1.2999999999999998</v>
-      </c>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1024,9 +991,7 @@
       <c r="H16" s="2">
         <v>30</v>
       </c>
-      <c r="I16" s="11">
-        <v>3</v>
-      </c>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -1051,9 +1016,7 @@
       <c r="H17" s="3">
         <v>40</v>
       </c>
-      <c r="I17" s="12">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1080,9 +1043,7 @@
       <c r="H18" s="1">
         <v>80</v>
       </c>
-      <c r="I18" s="10">
-        <v>1.5999999999999996</v>
-      </c>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1107,9 +1068,7 @@
       <c r="H19" s="2">
         <v>70</v>
       </c>
-      <c r="I19" s="11">
-        <v>0.90000000000000036</v>
-      </c>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -1134,9 +1093,7 @@
       <c r="H20" s="2">
         <v>30</v>
       </c>
-      <c r="I20" s="11">
-        <v>0.19999999999999929</v>
-      </c>
+      <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1161,9 +1118,7 @@
       <c r="H21" s="3">
         <v>40</v>
       </c>
-      <c r="I21" s="12">
-        <v>-0.5</v>
-      </c>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1190,9 +1145,7 @@
       <c r="H22" s="1">
         <v>80</v>
       </c>
-      <c r="I22" s="10">
-        <v>-1.1999999999999993</v>
-      </c>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1217,9 +1170,7 @@
       <c r="H23" s="2">
         <v>70</v>
       </c>
-      <c r="I23" s="11">
-        <v>-1.9000000000000004</v>
-      </c>
+      <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1244,9 +1195,7 @@
       <c r="H24" s="2">
         <v>30</v>
       </c>
-      <c r="I24" s="11">
-        <v>-2.5999999999999996</v>
-      </c>
+      <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1271,9 +1220,7 @@
       <c r="H25" s="3">
         <v>40</v>
       </c>
-      <c r="I25" s="12">
-        <v>-3.3000000000000007</v>
-      </c>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1300,9 +1247,7 @@
       <c r="H26" s="1">
         <v>80</v>
       </c>
-      <c r="I26" s="10">
-        <v>-4</v>
-      </c>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -1327,9 +1272,7 @@
       <c r="H27" s="2">
         <v>70</v>
       </c>
-      <c r="I27" s="11">
-        <v>-4.6999999999999993</v>
-      </c>
+      <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1354,9 +1297,7 @@
       <c r="H28" s="2">
         <v>30</v>
       </c>
-      <c r="I28" s="11">
-        <v>-5.4</v>
-      </c>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
@@ -1381,9 +1322,7 @@
       <c r="H29" s="3">
         <v>40</v>
       </c>
-      <c r="I29" s="12">
-        <v>-6.1000000000000014</v>
-      </c>
+      <c r="I29" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Got rid of try except command.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICE\ICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B025EC-8097-45FC-AD15-F5C6A4800875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7349FD4-87E1-40E3-A636-2A39FBAA9F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{D6852908-AD57-44F1-8DA2-95DC3E542023}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Pon</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Godzina</t>
+  </si>
+  <si>
+    <t>Komentarze</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -254,9 +257,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +577,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +616,9 @@
       <c r="H1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="10"/>
+      <c r="I1" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -640,7 +645,7 @@
       <c r="H2" s="1">
         <v>80</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -665,7 +670,7 @@
       <c r="H3" s="2">
         <v>70</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -690,7 +695,7 @@
       <c r="H4" s="2">
         <v>30</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -715,7 +720,7 @@
       <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -742,7 +747,7 @@
       <c r="H6" s="1">
         <v>80</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -767,7 +772,7 @@
       <c r="H7" s="2">
         <v>70</v>
       </c>
-      <c r="I7" s="8"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -792,7 +797,7 @@
       <c r="H8" s="2">
         <v>30</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -817,7 +822,7 @@
       <c r="H9" s="3">
         <v>40</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -844,7 +849,7 @@
       <c r="H10" s="1">
         <v>80</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
@@ -869,7 +874,7 @@
       <c r="H11" s="2">
         <v>70</v>
       </c>
-      <c r="I11" s="8"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -894,7 +899,7 @@
       <c r="H12" s="2">
         <v>30</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -919,7 +924,7 @@
       <c r="H13" s="3">
         <v>40</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -946,7 +951,7 @@
       <c r="H14" s="1">
         <v>80</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -971,7 +976,7 @@
       <c r="H15" s="2">
         <v>70</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -996,7 +1001,7 @@
       <c r="H16" s="2">
         <v>30</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -1021,7 +1026,7 @@
       <c r="H17" s="3">
         <v>40</v>
       </c>
-      <c r="I17" s="9"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1048,7 +1053,7 @@
       <c r="H18" s="1">
         <v>80</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1073,7 +1078,7 @@
       <c r="H19" s="2">
         <v>70</v>
       </c>
-      <c r="I19" s="8"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -1098,7 +1103,7 @@
       <c r="H20" s="2">
         <v>30</v>
       </c>
-      <c r="I20" s="8"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1123,7 +1128,7 @@
       <c r="H21" s="3">
         <v>40</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1150,7 +1155,7 @@
       <c r="H22" s="1">
         <v>80</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1175,7 +1180,7 @@
       <c r="H23" s="2">
         <v>70</v>
       </c>
-      <c r="I23" s="8"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
@@ -1200,7 +1205,7 @@
       <c r="H24" s="2">
         <v>30</v>
       </c>
-      <c r="I24" s="8"/>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1225,7 +1230,7 @@
       <c r="H25" s="3">
         <v>40</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1252,7 +1257,7 @@
       <c r="H26" s="1">
         <v>80</v>
       </c>
-      <c r="I26" s="7"/>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
@@ -1277,7 +1282,7 @@
       <c r="H27" s="2">
         <v>70</v>
       </c>
-      <c r="I27" s="8"/>
+      <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
@@ -1302,7 +1307,7 @@
       <c r="H28" s="2">
         <v>30</v>
       </c>
-      <c r="I28" s="8"/>
+      <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
@@ -1327,7 +1332,7 @@
       <c r="H29" s="3">
         <v>40</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>

</xml_diff>

<commit_message>
Support for data from CSV added
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICE\ICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7349FD4-87E1-40E3-A636-2A39FBAA9F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133B074B-B138-44D6-9DD5-FB2DED96D1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{D6852908-AD57-44F1-8DA2-95DC3E542023}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6852908-AD57-44F1-8DA2-95DC3E542023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -243,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -255,7 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -576,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D33CDED-A91F-4C7B-8534-B0E0E58BD3F9}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,98 +623,98 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>0.375</v>
       </c>
       <c r="C2" s="7">
-        <v>3</v>
+        <v>-7</v>
       </c>
       <c r="D2" s="1">
-        <v>5</v>
+        <v>3.1</v>
       </c>
       <c r="E2" s="4">
-        <v>10</v>
+        <v>5.2</v>
       </c>
       <c r="F2" s="1">
-        <v>990</v>
+        <v>1006</v>
       </c>
       <c r="G2" s="4">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>0.625</v>
       </c>
       <c r="C3" s="8">
-        <v>2</v>
+        <v>-15</v>
       </c>
       <c r="D3" s="2">
-        <v>4</v>
-      </c>
-      <c r="E3" s="11">
-        <v>12</v>
+        <v>8.9</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5</v>
       </c>
       <c r="F3" s="2">
         <v>990</v>
       </c>
-      <c r="G3" s="11">
-        <v>46</v>
+      <c r="G3" s="2">
+        <v>53</v>
       </c>
       <c r="H3" s="2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>0.75</v>
       </c>
       <c r="C4" s="8">
-        <v>1</v>
+        <v>-13</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11">
-        <v>13</v>
+        <v>6.2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.9000000000000004</v>
       </c>
       <c r="F4" s="2">
-        <v>989</v>
-      </c>
-      <c r="G4" s="11">
-        <v>24</v>
+        <v>980</v>
+      </c>
+      <c r="G4" s="2">
+        <v>50</v>
       </c>
       <c r="H4" s="2">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>0.875</v>
       </c>
       <c r="C5" s="9">
-        <v>1</v>
+        <v>-8</v>
       </c>
       <c r="D5" s="3">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="E5" s="6">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="G5" s="6">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" s="3">
         <v>40</v>
@@ -726,101 +725,101 @@
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>0.375</v>
       </c>
       <c r="C6" s="7">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="E6" s="4">
-        <v>16.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F6" s="1">
-        <v>990.5</v>
+        <v>1005</v>
       </c>
       <c r="G6" s="4">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H6" s="1">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>0.625</v>
       </c>
       <c r="C7" s="8">
-        <v>4.3</v>
+        <v>-12</v>
       </c>
       <c r="D7" s="2">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E7" s="11">
-        <v>18.100000000000001</v>
+        <v>5.6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4.9000000000000004</v>
       </c>
       <c r="F7" s="2">
-        <v>990.7</v>
-      </c>
-      <c r="G7" s="11">
-        <v>45.2</v>
+        <v>1004</v>
+      </c>
+      <c r="G7" s="2">
+        <v>49</v>
       </c>
       <c r="H7" s="2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>0.75</v>
       </c>
       <c r="C8" s="8">
-        <v>3.6</v>
+        <v>-12</v>
       </c>
       <c r="D8" s="2">
-        <v>8.6</v>
-      </c>
-      <c r="E8" s="11">
-        <v>19.7</v>
+        <v>4.8</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5.0999999999999996</v>
       </c>
       <c r="F8" s="2">
-        <v>990.9</v>
-      </c>
-      <c r="G8" s="11">
-        <v>45.4</v>
+        <v>984</v>
+      </c>
+      <c r="G8" s="2">
+        <v>37</v>
       </c>
       <c r="H8" s="2">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>0.875</v>
       </c>
       <c r="C9" s="9">
-        <v>2.9</v>
+        <v>-7</v>
       </c>
       <c r="D9" s="3">
-        <v>7.9</v>
+        <v>1.7</v>
       </c>
       <c r="E9" s="6">
-        <v>21.3</v>
+        <v>5.2</v>
       </c>
       <c r="F9" s="3">
-        <v>991.1</v>
+        <v>995</v>
       </c>
       <c r="G9" s="6">
-        <v>45.6</v>
+        <v>54</v>
       </c>
       <c r="H9" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -828,101 +827,101 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>0.375</v>
       </c>
       <c r="C10" s="7">
-        <v>2.2000000000000002</v>
+        <v>-6</v>
       </c>
       <c r="D10" s="1">
-        <v>7.2</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="4">
-        <v>22.9</v>
+        <v>5.4</v>
       </c>
       <c r="F10" s="1">
-        <v>991.3</v>
+        <v>1014</v>
       </c>
       <c r="G10" s="4">
-        <v>45.8</v>
+        <v>48</v>
       </c>
       <c r="H10" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>0.625</v>
       </c>
       <c r="C11" s="8">
+        <v>-8</v>
+      </c>
+      <c r="D11" s="2">
         <v>1.5</v>
       </c>
-      <c r="D11" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="E11" s="11">
-        <v>24.5</v>
+      <c r="E11" s="2">
+        <v>5.3</v>
       </c>
       <c r="F11" s="2">
-        <v>991.5</v>
-      </c>
-      <c r="G11" s="11">
-        <v>46</v>
+        <v>1012</v>
+      </c>
+      <c r="G11" s="2">
+        <v>49</v>
       </c>
       <c r="H11" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>0.75</v>
       </c>
       <c r="C12" s="8">
-        <v>0.79999999999999982</v>
+        <v>-7</v>
       </c>
       <c r="D12" s="2">
-        <v>5.8</v>
-      </c>
-      <c r="E12" s="11">
-        <v>26.1</v>
+        <v>0.8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5.3</v>
       </c>
       <c r="F12" s="2">
-        <v>991.7</v>
-      </c>
-      <c r="G12" s="11">
-        <v>46.2</v>
+        <v>983</v>
+      </c>
+      <c r="G12" s="2">
+        <v>36</v>
       </c>
       <c r="H12" s="2">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>0.875</v>
       </c>
       <c r="C13" s="9">
-        <v>9.9999999999999645E-2</v>
+        <v>-5</v>
       </c>
       <c r="D13" s="3">
-        <v>5.0999999999999996</v>
+        <v>-1.7</v>
       </c>
       <c r="E13" s="6">
-        <v>27.7</v>
+        <v>5.6</v>
       </c>
       <c r="F13" s="3">
-        <v>991.9</v>
+        <v>1004</v>
       </c>
       <c r="G13" s="6">
-        <v>46.4</v>
+        <v>55</v>
       </c>
       <c r="H13" s="3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I13" s="3"/>
     </row>
@@ -930,98 +929,98 @@
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>0.375</v>
       </c>
       <c r="C14" s="7">
-        <v>-0.59999999999999964</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>4.4000000000000004</v>
+        <v>-7.6</v>
       </c>
       <c r="E14" s="4">
-        <v>29.3</v>
+        <v>5.8</v>
       </c>
       <c r="F14" s="1">
-        <v>992.1</v>
+        <v>1002</v>
       </c>
       <c r="G14" s="4">
-        <v>46.6</v>
+        <v>46</v>
       </c>
       <c r="H14" s="1">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="14">
+      <c r="B15" s="13">
         <v>0.625</v>
       </c>
       <c r="C15" s="8">
-        <v>-1.2999999999999998</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="E15" s="11">
-        <v>30.9</v>
+        <v>-4.5</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6.1</v>
       </c>
       <c r="F15" s="2">
-        <v>992.3</v>
-      </c>
-      <c r="G15" s="11">
-        <v>46.8</v>
+        <v>1003</v>
+      </c>
+      <c r="G15" s="2">
+        <v>43</v>
       </c>
       <c r="H15" s="2">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>0.75</v>
       </c>
       <c r="C16" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2">
-        <v>13</v>
-      </c>
-      <c r="E16" s="11">
-        <v>32.5</v>
+        <v>-6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>6.2</v>
       </c>
       <c r="F16" s="2">
-        <v>992.5</v>
-      </c>
-      <c r="G16" s="11">
-        <v>47</v>
+        <v>983</v>
+      </c>
+      <c r="G16" s="2">
+        <v>41</v>
       </c>
       <c r="H16" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>0.875</v>
       </c>
       <c r="C17" s="9">
-        <v>2.2999999999999998</v>
+        <v>0</v>
       </c>
       <c r="D17" s="3">
-        <v>12.3</v>
+        <v>-8.1</v>
       </c>
       <c r="E17" s="6">
-        <v>34.1</v>
+        <v>6.4</v>
       </c>
       <c r="F17" s="3">
-        <v>992.7</v>
+        <v>999</v>
       </c>
       <c r="G17" s="6">
-        <v>47.2</v>
+        <v>47</v>
       </c>
       <c r="H17" s="3">
         <v>40</v>
@@ -1032,48 +1031,48 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="12">
         <v>0.375</v>
       </c>
       <c r="C18" s="7">
-        <v>1.5999999999999996</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
-        <v>11.6</v>
+        <v>-5.2</v>
       </c>
       <c r="E18" s="4">
-        <v>35.700000000000003</v>
+        <v>6.5</v>
       </c>
       <c r="F18" s="1">
-        <v>992.9</v>
+        <v>1005</v>
       </c>
       <c r="G18" s="4">
-        <v>47.4</v>
+        <v>56</v>
       </c>
       <c r="H18" s="1">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <v>0.625</v>
       </c>
       <c r="C19" s="8">
-        <v>0.90000000000000036</v>
+        <v>-1</v>
       </c>
       <c r="D19" s="2">
-        <v>10.9</v>
-      </c>
-      <c r="E19" s="11">
-        <v>37.299999999999997</v>
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="E19" s="2">
+        <v>6.6</v>
       </c>
       <c r="F19" s="2">
-        <v>993.1</v>
-      </c>
-      <c r="G19" s="11">
-        <v>47.6</v>
+        <v>994</v>
+      </c>
+      <c r="G19" s="2">
+        <v>53</v>
       </c>
       <c r="H19" s="2">
         <v>70</v>
@@ -1082,51 +1081,51 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <v>0.75</v>
       </c>
       <c r="C20" s="8">
-        <v>0.19999999999999929</v>
+        <v>-1</v>
       </c>
       <c r="D20" s="2">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="E20" s="11">
-        <v>38.9</v>
+        <v>-3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>6.6</v>
       </c>
       <c r="F20" s="2">
-        <v>993.3</v>
-      </c>
-      <c r="G20" s="11">
-        <v>47.8</v>
+        <v>1010</v>
+      </c>
+      <c r="G20" s="2">
+        <v>57</v>
       </c>
       <c r="H20" s="2">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>0.875</v>
       </c>
       <c r="C21" s="9">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>9.5</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="E21" s="6">
-        <v>40.5</v>
+        <v>6.8</v>
       </c>
       <c r="F21" s="3">
-        <v>993.5</v>
+        <v>1004</v>
       </c>
       <c r="G21" s="6">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H21" s="3">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="I21" s="3"/>
     </row>
@@ -1134,101 +1133,101 @@
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <v>0.375</v>
       </c>
       <c r="C22" s="7">
-        <v>-1.1999999999999993</v>
+        <v>-2</v>
       </c>
       <c r="D22" s="1">
-        <v>8.8000000000000007</v>
+        <v>-1.5</v>
       </c>
       <c r="E22" s="4">
-        <v>42.1</v>
+        <v>6.8</v>
       </c>
       <c r="F22" s="1">
-        <v>993.7</v>
+        <v>1010</v>
       </c>
       <c r="G22" s="4">
-        <v>48.2</v>
+        <v>36</v>
       </c>
       <c r="H22" s="1">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="14">
+      <c r="B23" s="13">
         <v>0.625</v>
       </c>
       <c r="C23" s="8">
-        <v>-1.9000000000000004</v>
+        <v>-4</v>
       </c>
       <c r="D23" s="2">
-        <v>8.1</v>
-      </c>
-      <c r="E23" s="11">
-        <v>43.7</v>
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>6.7</v>
       </c>
       <c r="F23" s="2">
-        <v>993.9</v>
-      </c>
-      <c r="G23" s="11">
-        <v>48.4</v>
+        <v>1000</v>
+      </c>
+      <c r="G23" s="2">
+        <v>44</v>
       </c>
       <c r="H23" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="14">
+      <c r="B24" s="13">
         <v>0.75</v>
       </c>
       <c r="C24" s="8">
-        <v>-2.5999999999999996</v>
+        <v>-3</v>
       </c>
       <c r="D24" s="2">
-        <v>7.4</v>
-      </c>
-      <c r="E24" s="11">
-        <v>45.3</v>
+        <v>0.9</v>
+      </c>
+      <c r="E24" s="2">
+        <v>6.7</v>
       </c>
       <c r="F24" s="2">
-        <v>994.1</v>
-      </c>
-      <c r="G24" s="11">
-        <v>48.6</v>
+        <v>999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>40</v>
       </c>
       <c r="H24" s="2">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>0.875</v>
       </c>
       <c r="C25" s="9">
-        <v>-3.3000000000000007</v>
+        <v>-3</v>
       </c>
       <c r="D25" s="3">
-        <v>6.6999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E25" s="6">
-        <v>46.9</v>
+        <v>6.7</v>
       </c>
       <c r="F25" s="3">
-        <v>994.3</v>
+        <v>999</v>
       </c>
       <c r="G25" s="6">
-        <v>48.8</v>
+        <v>57</v>
       </c>
       <c r="H25" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I25" s="3"/>
     </row>
@@ -1236,23 +1235,23 @@
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <v>0.375</v>
       </c>
       <c r="C26" s="7">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="D26" s="1">
-        <v>6</v>
+        <v>1.3</v>
       </c>
       <c r="E26" s="4">
-        <v>48.5</v>
+        <v>6.6</v>
       </c>
       <c r="F26" s="1">
-        <v>994.5</v>
+        <v>985</v>
       </c>
       <c r="G26" s="4">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H26" s="1">
         <v>80</v>
@@ -1261,81 +1260,81 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="14">
+      <c r="B27" s="13">
         <v>0.625</v>
       </c>
       <c r="C27" s="8">
-        <v>-4.6999999999999993</v>
+        <v>-10</v>
       </c>
       <c r="D27" s="2">
-        <v>5.3000000000000007</v>
-      </c>
-      <c r="E27" s="11">
-        <v>50.1</v>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E27" s="2">
+        <v>6.5</v>
       </c>
       <c r="F27" s="2">
-        <v>994.7</v>
-      </c>
-      <c r="G27" s="11">
-        <v>49.2</v>
+        <v>993</v>
+      </c>
+      <c r="G27" s="2">
+        <v>59</v>
       </c>
       <c r="H27" s="2">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="14">
+      <c r="B28" s="13">
         <v>0.75</v>
       </c>
       <c r="C28" s="8">
-        <v>-5.4</v>
+        <v>-10</v>
       </c>
       <c r="D28" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E28" s="11">
-        <v>51.7</v>
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <v>6.4</v>
       </c>
       <c r="F28" s="2">
-        <v>994.9</v>
-      </c>
-      <c r="G28" s="11">
-        <v>49.4</v>
+        <v>1011</v>
+      </c>
+      <c r="G28" s="2">
+        <v>47</v>
       </c>
       <c r="H28" s="2">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>0.875</v>
       </c>
       <c r="C29" s="9">
-        <v>-6.1000000000000014</v>
+        <v>-8</v>
       </c>
       <c r="D29" s="3">
-        <v>3.8999999999999986</v>
+        <v>2.9</v>
       </c>
       <c r="E29" s="6">
-        <v>53.3</v>
+        <v>6.4</v>
       </c>
       <c r="F29" s="3">
-        <v>995.1</v>
+        <v>980</v>
       </c>
       <c r="G29" s="6">
-        <v>49.6</v>
+        <v>58</v>
       </c>
       <c r="H29" s="3">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
+      <c r="B30" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Import options tasks finalized
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICE\ICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133B074B-B138-44D6-9DD5-FB2DED96D1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232C8A8F-DAD5-4DB1-91B5-A567DBD7A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6852908-AD57-44F1-8DA2-95DC3E542023}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Pon</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>Wt.</t>
   </si>
@@ -83,7 +80,7 @@
     <t>Godzina</t>
   </si>
   <si>
-    <t>Komentarze</t>
+    <t>Pon.</t>
   </si>
 </sst>
 </file>
@@ -119,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -189,17 +186,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -243,22 +229,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D33CDED-A91F-4C7B-8534-B0E0E58BD3F9}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,46 +572,42 @@
     <col min="6" max="6" width="22.85546875" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>0.375</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>-7</v>
       </c>
       <c r="D2" s="1">
@@ -644,14 +625,15 @@
       <c r="H2" s="1">
         <v>60</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="13">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="12">
         <v>0.625</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>-15</v>
       </c>
       <c r="D3" s="2">
@@ -669,14 +651,15 @@
       <c r="H3" s="2">
         <v>90</v>
       </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="13">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="12">
         <v>0.75</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>-13</v>
       </c>
       <c r="D4" s="2">
@@ -694,41 +677,41 @@
       <c r="H4" s="2">
         <v>70</v>
       </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="14">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="13">
         <v>0.875</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>-8</v>
       </c>
       <c r="D5" s="3">
         <v>4.2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>5</v>
       </c>
       <c r="F5" s="3">
         <v>988</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>44</v>
       </c>
       <c r="H5" s="3">
         <v>40</v>
       </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="12">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11">
         <v>0.375</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>-7</v>
       </c>
       <c r="D6" s="1">
@@ -746,14 +729,15 @@
       <c r="H6" s="1">
         <v>65</v>
       </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="13">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="12">
         <v>0.625</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>-12</v>
       </c>
       <c r="D7" s="2">
@@ -771,14 +755,15 @@
       <c r="H7" s="2">
         <v>90</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="13">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="12">
         <v>0.75</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>-12</v>
       </c>
       <c r="D8" s="2">
@@ -796,41 +781,41 @@
       <c r="H8" s="2">
         <v>80</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="14">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="13">
         <v>0.875</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>-7</v>
       </c>
       <c r="D9" s="3">
         <v>1.7</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>5.2</v>
       </c>
       <c r="F9" s="3">
         <v>995</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>54</v>
       </c>
       <c r="H9" s="3">
         <v>30</v>
       </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11">
         <v>0.375</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>-6</v>
       </c>
       <c r="D10" s="1">
@@ -848,14 +833,15 @@
       <c r="H10" s="1">
         <v>50</v>
       </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="13">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="12">
         <v>0.625</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>-8</v>
       </c>
       <c r="D11" s="2">
@@ -873,14 +859,15 @@
       <c r="H11" s="2">
         <v>60</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="13">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12">
         <v>0.75</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>-7</v>
       </c>
       <c r="D12" s="2">
@@ -898,41 +885,41 @@
       <c r="H12" s="2">
         <v>55</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="14">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13">
         <v>0.875</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>-5</v>
       </c>
       <c r="D13" s="3">
         <v>-1.7</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>5.6</v>
       </c>
       <c r="F13" s="3">
         <v>1004</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>55</v>
       </c>
       <c r="H13" s="3">
         <v>20</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="12">
+        <v>2</v>
+      </c>
+      <c r="B14" s="11">
         <v>0.375</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0</v>
       </c>
       <c r="D14" s="1">
@@ -950,14 +937,15 @@
       <c r="H14" s="1">
         <v>10</v>
       </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="13">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="12">
         <v>0.625</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>0</v>
       </c>
       <c r="D15" s="2">
@@ -975,14 +963,15 @@
       <c r="H15" s="2">
         <v>30</v>
       </c>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="13">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="12">
         <v>0.75</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>0</v>
       </c>
       <c r="D16" s="2">
@@ -1000,41 +989,41 @@
       <c r="H16" s="2">
         <v>20</v>
       </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="14">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="13">
         <v>0.875</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>0</v>
       </c>
       <c r="D17" s="3">
         <v>-8.1</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>6.4</v>
       </c>
       <c r="F17" s="3">
         <v>999</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>47</v>
       </c>
       <c r="H17" s="3">
         <v>40</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="12">
+        <v>3</v>
+      </c>
+      <c r="B18" s="11">
         <v>0.375</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>0</v>
       </c>
       <c r="D18" s="1">
@@ -1052,14 +1041,15 @@
       <c r="H18" s="1">
         <v>30</v>
       </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="13">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="12">
         <v>0.625</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>-1</v>
       </c>
       <c r="D19" s="2">
@@ -1077,14 +1067,15 @@
       <c r="H19" s="2">
         <v>70</v>
       </c>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="13">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="12">
         <v>0.75</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>-1</v>
       </c>
       <c r="D20" s="2">
@@ -1102,41 +1093,41 @@
       <c r="H20" s="2">
         <v>80</v>
       </c>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="14">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="13">
         <v>0.875</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>0</v>
       </c>
       <c r="D21" s="3">
         <v>-4.0999999999999996</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>6.8</v>
       </c>
       <c r="F21" s="3">
         <v>1004</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>41</v>
       </c>
       <c r="H21" s="3">
         <v>60</v>
       </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="12">
+        <v>4</v>
+      </c>
+      <c r="B22" s="11">
         <v>0.375</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>-2</v>
       </c>
       <c r="D22" s="1">
@@ -1154,14 +1145,15 @@
       <c r="H22" s="1">
         <v>50</v>
       </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="13">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="12">
         <v>0.625</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>-4</v>
       </c>
       <c r="D23" s="2">
@@ -1179,14 +1171,15 @@
       <c r="H23" s="2">
         <v>60</v>
       </c>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="13">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="12">
         <v>0.75</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>-3</v>
       </c>
       <c r="D24" s="2">
@@ -1204,41 +1197,41 @@
       <c r="H24" s="2">
         <v>55</v>
       </c>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="14">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="13">
         <v>0.875</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>-3</v>
       </c>
       <c r="D25" s="3">
         <v>0</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>6.7</v>
       </c>
       <c r="F25" s="3">
         <v>999</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>57</v>
       </c>
       <c r="H25" s="3">
         <v>30</v>
       </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="12">
+        <v>5</v>
+      </c>
+      <c r="B26" s="11">
         <v>0.375</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>-6</v>
       </c>
       <c r="D26" s="1">
@@ -1256,14 +1249,15 @@
       <c r="H26" s="1">
         <v>80</v>
       </c>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="13">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="12">
         <v>0.625</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>-10</v>
       </c>
       <c r="D27" s="2">
@@ -1281,14 +1275,15 @@
       <c r="H27" s="2">
         <v>90</v>
       </c>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="13">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="12">
         <v>0.75</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>-10</v>
       </c>
       <c r="D28" s="2">
@@ -1306,38 +1301,39 @@
       <c r="H28" s="2">
         <v>90</v>
       </c>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="14">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="13">
         <v>0.875</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>-8</v>
       </c>
       <c r="D29" s="3">
         <v>2.9</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>6.4</v>
       </c>
       <c r="F29" s="3">
         <v>980</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>58</v>
       </c>
       <c r="H29" s="3">
         <v>80</v>
       </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>